<commit_message>
pushing the updated code
</commit_message>
<xml_diff>
--- a/uploads/case study demo.xlsx
+++ b/uploads/case study demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vedanth/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BDCCE7-B715-3F41-BA96-527FC0D43A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0E92C7-CCFD-CB44-A0C5-29CC45BC83DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{EC245EB4-59FD-474E-AD82-E490B36C14E7}"/>
+    <workbookView xWindow="1360" yWindow="760" windowWidth="28040" windowHeight="17260" xr2:uid="{EC245EB4-59FD-474E-AD82-E490B36C14E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>vedanth</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Last Name</t>
+  </si>
+  <si>
+    <t>poonacha</t>
+  </si>
+  <si>
+    <t>terry.poonacha@gmail.com</t>
+  </si>
+  <si>
+    <t>Terry</t>
   </si>
 </sst>
 </file>
@@ -436,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989E8D9F-CBD7-EC4E-850B-F8BFABFC59B3}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,9 +475,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{3BB7C5B6-F871-8949-87C9-22EFD8141ADD}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{ACC28E59-7410-4546-8176-BB2BB4816732}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>